<commit_message>
1.3.2.5 release; bugfixes, renames
</commit_message>
<xml_diff>
--- a/latest strings.xlsx
+++ b/latest strings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkC#\Ei_Dimension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F45CBC4-68C6-4187-A025-18BA93BEF947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0822ABA-FC4F-41E0-9C95-C247AC97FEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7725" yWindow="4335" windowWidth="14790" windowHeight="14940" xr2:uid="{15C89055-9C32-492D-BB65-CCF0B90D7398}"/>
   </bookViews>
@@ -56,35 +56,46 @@
     <t>PlateCustomization_FinalizedZPosition</t>
   </si>
   <si>
-    <t>Final Z Position</t>
-  </si>
-  <si>
     <t>PlateCustomization_InitialZPosition</t>
   </si>
   <si>
-    <t>Initial Z Position</t>
-  </si>
-  <si>
     <t>PlateCustomization_ZStep</t>
   </si>
   <si>
-    <t>Motor Step</t>
-  </si>
-  <si>
     <t>PlateCustomization_TunePlate</t>
   </si>
   <si>
-    <t>Start Plate Tuning</t>
+    <t>Gap Steps</t>
+  </si>
+  <si>
+    <t>Downstroke Steps</t>
+  </si>
+  <si>
+    <t>Upstroke Steps</t>
+  </si>
+  <si>
+    <t>Find Plate Depth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,8 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +442,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +471,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -466,35 +479,36 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>